<commit_message>
(Balan) Pump -> Balan の通信プロトコルを検討 #11
</commit_message>
<xml_diff>
--- a/DOC/Balan.xlsx
+++ b/DOC/Balan.xlsx
@@ -2,15 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F526FA-0770-49CE-9B31-E2AEAE48DB72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9151228-C51A-48BA-B42A-F24338B967DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14916" yWindow="4224" windowWidth="26568" windowHeight="18540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8370" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="パーツ一覧" sheetId="1" r:id="rId1"/>
     <sheet name="I2C_概要" sheetId="4" r:id="rId2"/>
     <sheet name="I2C_レジスタ一覧" sheetId="2" r:id="rId3"/>
+    <sheet name="通信プロトコル" sheetId="5" r:id="rId4"/>
+    <sheet name="ポンチ絵" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">I2C_レジスタ一覧!$C$4:$I$103</definedName>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="335">
   <si>
     <t>パーツ一覧</t>
   </si>
@@ -1974,6 +1976,417 @@
   </si>
   <si>
     <t>RM0316 リファレンスマニュアル</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■全体構成</t>
+    <rPh sb="1" eb="3">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[0]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[1]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[2]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Group Address</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Brick Address</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Reset</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Brightness</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[3]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data3</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[4]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[5]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Step Timing</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Is Repeat</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Pattern Id</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Set Pattern</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Set Brightness</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Register Type</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>凡例</t>
+    <rPh sb="0" eb="2">
+      <t>ハンレイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>値域</t>
+    <rPh sb="0" eb="2">
+      <t>チイキ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Command Type</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Brick Type</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0～15
+0 : 最小 / 15 : 最大</t>
+    <rPh sb="9" eb="11">
+      <t>サイショウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>サイダイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* チェックサムはエラーレートが低そう、かつデバッグしにくいので省略。</t>
+    <rPh sb="16" eb="17">
+      <t>ヒク</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ショウリャク</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■Pump → Balan (I2C)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>↑</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■PC → Pump (UART)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0x70～0x77 : 個別指定
+0xFF : ブロードキャスト</t>
+    <rPh sb="12" eb="14">
+      <t>コベツ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>通信プロトコル</t>
+    <rPh sb="0" eb="2">
+      <t>ツウシン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>I2C アドレス値域は固定</t>
+    <rPh sb="8" eb="10">
+      <t>チイキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>コテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>I2C アドレス値域は変更可能 (仮確定)</t>
+    <rPh sb="8" eb="10">
+      <t>チイキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カリ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カクテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Address1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Address2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* Balan は Brick を持っているか知っている必要があるので Register Type コマンドは必須。</t>
+    <rPh sb="17" eb="18">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ヒッス</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* Pump 自体は Brick 構成に関する情報を何も保持しない。単なる UART to I2C の土管として使用する。</t>
+    <rPh sb="7" eb="9">
+      <t>ジタイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウセイ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>タン</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ドカン</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* コマンドは "@send aabbccdd…" のみで、生データを 16 進数で直接指定して送信。</t>
+    <rPh sb="30" eb="31">
+      <t>ナマ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>シンスウ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>チョクセツ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ソウシン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■サンプルコマンド</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@send 607000</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>グループ 0、部品 0 をリセット</t>
+    <rPh sb="7" eb="9">
+      <t>ブヒン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@send 60700100</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>グループ 0、部品 0、草を登録</t>
+    <rPh sb="7" eb="9">
+      <t>ブヒン</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>クサ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>トウロク</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@send 607002000000</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@send 60700315</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>グループ 0、部品 0、輝度 15 を指定</t>
+    <rPh sb="7" eb="9">
+      <t>ブヒン</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>キド</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>グループ 0、部品 0、パターン 0、周期 0、リピート無　を指定</t>
+    <rPh sb="7" eb="9">
+      <t>ブヒン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>シュウキ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ナシ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* データ長はコマンド種別によって一意に定まるので省略。可変長。</t>
+    <rPh sb="5" eb="6">
+      <t>チョウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>イチイ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>サダ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ショウリャク</t>
+    </rPh>
+    <rPh sb="28" eb="31">
+      <t>カヘンチョウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0x00 : Reset
+0x01 : RegisterType
+0x02 : SetPattern
+0x03 : SetBrightness</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0xFF : Default
+0x00 : Grass
+0x01 : Tree
+0x02 : House
+0x03 : Tile</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■エラーハンドリングなど</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* 現状は特に用意しない。</t>
+    <rPh sb="2" eb="4">
+      <t>ゲンジョウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>トク</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヨウイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* タイムアウトはあった方がいい気がするが…とりあえず受信が正しくできるようになってから。</t>
+    <rPh sb="12" eb="13">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ジュシン</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>タダ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0x60～0x67 : 個別指定</t>
+    <rPh sb="12" eb="14">
+      <t>コベツ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シテイ</t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -2062,7 +2475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2166,11 +2579,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2265,6 +2695,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2575,10 +3018,1046 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="40" name="グループ化 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5162A9D6-6FD9-4D80-BE04-F1E0F78EB963}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="952500" y="1099038"/>
+          <a:ext cx="4572000" cy="3480289"/>
+          <a:chOff x="967154" y="1090246"/>
+          <a:chExt cx="4642338" cy="3452446"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="正方形/長方形 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D49B4EC5-9A54-4E70-81D0-8D52659B14D7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="967154" y="1090246"/>
+            <a:ext cx="4642338" cy="3452446"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="正方形/長方形 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED2DA4DA-2B5A-4C1D-B070-381AD7F62E71}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2989384" y="3006970"/>
+            <a:ext cx="773723" cy="363416"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>Balan</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="正方形/長方形 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0293DE-4168-427B-980F-DBE1EC683A68}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2995247" y="3915509"/>
+            <a:ext cx="773723" cy="357552"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>Brick</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="正方形/長方形 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AE0E932-31AC-4E09-9DF1-1E1D444C3198}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2901461" y="1271955"/>
+            <a:ext cx="773722" cy="363415"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>PC</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="正方形/長方形 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB2AC42-2A1C-43A0-82EE-69F6145AC800}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2901461" y="2180492"/>
+            <a:ext cx="773722" cy="363416"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>Pump</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="正方形/長方形 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A67AEC42-E91C-4A04-B718-BC2D3857CD8A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2901461" y="3089032"/>
+            <a:ext cx="773722" cy="363415"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>Balan</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="正方形/長方形 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7756C307-F1CC-43B5-A1E6-9225258FD1B4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2901461" y="4003431"/>
+            <a:ext cx="773722" cy="357554"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>Brick</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="直線コネクタ 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{083B91ED-4B4D-4D5A-99BD-FCAF47BC3E88}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="4" idx="2"/>
+            <a:endCxn id="6" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3288322" y="1635370"/>
+            <a:ext cx="0" cy="545122"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="11" name="直線コネクタ 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CCF7E0A-AF73-4AF3-A94F-F0543EAE0F4D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="6" idx="2"/>
+            <a:endCxn id="7" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3288322" y="2543908"/>
+            <a:ext cx="0" cy="545124"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="14" name="直線コネクタ 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F074DC0A-A34D-4DEE-B9F4-02E6E67816F9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="7" idx="2"/>
+            <a:endCxn id="8" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3288322" y="3452447"/>
+            <a:ext cx="0" cy="550984"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="18" name="直線コネクタ 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA83118-F370-4279-BDB8-99E19F125997}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="7" idx="1"/>
+            <a:endCxn id="21" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="2127738" y="3270739"/>
+            <a:ext cx="773723" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="正方形/長方形 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{462815EC-B442-410A-AA58-121219A5CDAE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1354016" y="3089032"/>
+            <a:ext cx="773722" cy="363415"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>PC</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="27" name="右中かっこ 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA4C683-FF98-4D2B-BD2B-CF5207255BE7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4062046" y="3815862"/>
+            <a:ext cx="193431" cy="545123"/>
+          </a:xfrm>
+          <a:prstGeom prst="rightBrace">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 44697"/>
+              <a:gd name="adj2" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="右中かっこ 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA06E0D-38B2-45F4-B042-040D263A42CC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4062046" y="2907323"/>
+            <a:ext cx="193431" cy="545124"/>
+          </a:xfrm>
+          <a:prstGeom prst="rightBrace">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 44697"/>
+              <a:gd name="adj2" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="大かっこ 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F157ABF3-0FB7-482D-A0E8-A86600090306}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1160585" y="2907323"/>
+            <a:ext cx="1160584" cy="726830"/>
+          </a:xfrm>
+          <a:prstGeom prst="bracketPair">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="テキスト ボックス 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB8FE58-7DAF-4C39-95F3-2CF48509D620}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3481754" y="1714598"/>
+            <a:ext cx="1067665" cy="325217"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>UART</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+              <a:t> or BLE</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="テキスト ボックス 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A806B390-3474-4B11-B0F5-CCFF217447D8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3481754" y="2582107"/>
+            <a:ext cx="423962" cy="325217"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>I2C</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="テキスト ボックス 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{492A520A-C6F8-489C-89EF-A6D40EBE0FB6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3481754" y="3490644"/>
+            <a:ext cx="423962" cy="325217"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>I2C</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="テキスト ボックス 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F313BA7-5FB0-4E45-8ADD-080D8EEA64E9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2127738" y="3452446"/>
+            <a:ext cx="874598" cy="558102"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>UART</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+              <a:t>デバッグ用</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="テキスト ボックス 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14F531E5-82ED-43D9-92BD-BED6473E4930}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4396154" y="3015860"/>
+            <a:ext cx="1115626" cy="325217"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>MAX 8 (0</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+              <a:t>～</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>7)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="テキスト ボックス 37">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EB91A1D-76A6-43F2-BA8D-6A40F7346F0F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4378570" y="3924399"/>
+            <a:ext cx="1115626" cy="325217"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>MAX 8 (0</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+              <a:t>～</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>7)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007-2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2586,143 +4065,49 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="ユーザー定義 1">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
+        <a:latin typeface="Meiryo UI"/>
+        <a:ea typeface="Meiryo UI"/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
+        <a:latin typeface="Meiryo UI"/>
+        <a:ea typeface="Meiryo UI"/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007-2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2731,93 +4116,110 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -4195,7 +5597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8D4F10-6A18-43C0-B2B5-69608E1CD86C}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6047,4 +7449,324 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E918656-40EA-4B26-9256-33A6570B993C}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="2.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="4" customWidth="1"/>
+    <col min="7" max="9" width="16.109375" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B3" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C4" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C5" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B7" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C8" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C9" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C10" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D12" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>289</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D13" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D14" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D15" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D16" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D17" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D20" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="D21" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="D22" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
+      <c r="D23" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="72" x14ac:dyDescent="0.4">
+      <c r="D24" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="D25" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B28" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D29" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D30" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D31" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D32" s="38" t="s">
+        <v>325</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B35" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C36" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C37" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C437A82F-3511-4761-92A9-F95BE150123C}">
+  <dimension ref="E5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="2.77734375" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="34" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(Balan) Register, Reset コマンドの追加 #31
</commit_message>
<xml_diff>
--- a/DOC/Balan.xlsx
+++ b/DOC/Balan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB39B71-A006-4B8B-BEF1-9E11C11EDBB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC5AA25-A04B-4171-BAE3-EE8FCFF78E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21060" yWindow="4848" windowWidth="23268" windowHeight="17580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20124" yWindow="4992" windowWidth="19980" windowHeight="16344" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="パーツ一覧" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="338">
   <si>
     <t>パーツ一覧</t>
   </si>
@@ -2076,17 +2076,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>0x70～0x77 : 個別指定
-0xFF : ブロードキャスト</t>
-    <rPh sb="12" eb="14">
-      <t>コベツ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>シテイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>通信プロトコル</t>
     <rPh sb="0" eb="2">
       <t>ツウシン</t>
@@ -2094,35 +2083,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>I2C アドレス値域は固定</t>
-    <rPh sb="8" eb="10">
-      <t>チイキ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>コテイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>I2C アドレス値域は変更可能 (仮確定)</t>
-    <rPh sb="8" eb="10">
-      <t>チイキ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ヘンコウ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>カノウ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>カリ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>カクテイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Address1</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -2285,21 +2245,6 @@
     <rPh sb="28" eb="31">
       <t>カヘンチョウ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>0x00 : Reset
-0x01 : RegisterType
-0x02 : SetPattern
-0x03 : SetBrightness</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>0xFF : Default
-0x00 : Grass
-0x01 : Tree
-0x02 : House
-0x03 : Tile</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -2441,12 +2386,141 @@
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>0x00～0x07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> : 個別指定
+0xFF : ブロードキャスト</t>
+    </r>
+    <rPh sb="12" eb="14">
+      <t>コベツ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>HT16K33 のアドレスは隠蔽。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+I2C アドレス値域は固定</t>
+    </r>
+    <rPh sb="14" eb="16">
+      <t>インペイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>チイキ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>コテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>I2C アドレス値域は変更可能。 (仮確定)</t>
+    <rPh sb="8" eb="10">
+      <t>チイキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>カリ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>カクテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>★ユーザレベルからはここも隠蔽されるのでゲタ分の有無はどっちでもいいというのが結論。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>★最終的にはゲタ分は無しにしたい！(Pump 側で加算？）だがデバッグ用のために現状では Pump に情報を持たせたくない。</t>
+    <rPh sb="1" eb="4">
+      <t>サイシュウテキ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ブン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>カサン</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ゲンジョウ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0x00 : Reset
+0x01 : RegisterBrick
+0x02 : SetPattern
+0x03 : SetBrightness</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0x00 : Grass
+0x01 : Tree
+0x02 : House
+0x03 : Tile</t>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="游ゴシック"/>
@@ -2498,6 +2572,20 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
       <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
@@ -2660,7 +2748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2765,10 +2853,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5660,7 +5751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8D4F10-6A18-43C0-B2B5-69608E1CD86C}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5761,7 +5852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12935401-6BAD-42DF-866E-A7F43B1CDBF4}">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5948,7 +6039,7 @@
         <v>162</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.4">
@@ -5963,8 +6054,8 @@
       <c r="G14" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>334</v>
+      <c r="H14" s="38" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -6046,8 +6137,8 @@
       <c r="G19" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="H19" s="39" t="s">
-        <v>333</v>
+      <c r="H19" s="38" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.4">
@@ -7518,8 +7609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E918656-40EA-4B26-9256-33A6570B993C}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
@@ -7528,14 +7619,15 @@
     <col min="2" max="3" width="2.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="16.109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="24.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" style="4" customWidth="1"/>
-    <col min="7" max="9" width="16.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="16.109375" style="4" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
@@ -7545,12 +7637,12 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C4" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C5" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -7560,7 +7652,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C8" s="4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -7570,7 +7662,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C10" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -7595,10 +7687,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="D13" s="35" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F13" s="35" t="s">
         <v>301</v>
@@ -7696,15 +7788,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" ht="86.4" x14ac:dyDescent="0.4">
       <c r="D21" s="2" t="s">
         <v>283</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>311</v>
+        <v>333</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>335</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
@@ -7712,10 +7810,10 @@
         <v>284</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>310</v>
+        <v>331</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
@@ -7723,18 +7821,18 @@
         <v>301</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="72" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
       <c r="D24" s="2" t="s">
         <v>302</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>65</v>
@@ -7753,54 +7851,54 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B28" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D29" s="39" t="s">
+        <v>315</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D30" s="39" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D29" s="38" t="s">
+      <c r="F30" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="F29" s="4" t="s">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D31" s="39" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D30" s="38" t="s">
+      <c r="F31" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D32" s="39" t="s">
         <v>320</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D31" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D32" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B35" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C36" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C37" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(Balan) SetStepTiming コマンドの追加 #47
</commit_message>
<xml_diff>
--- a/DOC/Balan.xlsx
+++ b/DOC/Balan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC5AA25-A04B-4171-BAE3-EE8FCFF78E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28972B8-A699-4F56-AAFD-1ED7D59D5F68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20124" yWindow="4992" windowWidth="19980" windowHeight="16344" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3144" yWindow="3792" windowWidth="19932" windowHeight="18684" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="パーツ一覧" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="339">
   <si>
     <t>パーツ一覧</t>
   </si>
@@ -2513,6 +2513,10 @@
 0x01 : Tree
 0x02 : House
 0x03 : Tile</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Set Step Timing</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -7607,11 +7611,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E918656-40EA-4B26-9256-33A6570B993C}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
   <cols>
@@ -7772,132 +7774,148 @@
       <c r="I17" s="37"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D20" s="35" t="s">
+      <c r="D18" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D21" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E21" s="35" t="s">
         <v>300</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="86.4" x14ac:dyDescent="0.4">
-      <c r="D21" s="2" t="s">
+    <row r="22" spans="2:9" ht="86.4" x14ac:dyDescent="0.4">
+      <c r="D22" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="G21" s="40" t="s">
+      <c r="G22" s="40" t="s">
         <v>335</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H22" s="40" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
-      <c r="D22" s="2" t="s">
+    <row r="23" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="D23" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
-      <c r="D23" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
       <c r="D24" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
       <c r="D25" s="2" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>303</v>
+        <v>337</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B28" s="4" t="s">
+    <row r="26" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="D26" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B29" s="4" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D29" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D30" s="39" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D31" s="39" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D32" s="39" t="s">
+        <v>319</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D33" s="39" t="s">
         <v>320</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B36" s="4" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C36" s="4" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C37" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C37" s="4" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C38" s="4" t="s">
         <v>326</v>
       </c>
     </row>

</xml_diff>

<commit_message>
(Balan) StepTiming を 1byte から 2byte に変更 #47
</commit_message>
<xml_diff>
--- a/DOC/Balan.xlsx
+++ b/DOC/Balan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28972B8-A699-4F56-AAFD-1ED7D59D5F68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6D1EAE-8729-4F22-B245-EEF0A3E2A03D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3144" yWindow="3792" windowWidth="19932" windowHeight="18684" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10944" yWindow="3588" windowWidth="31620" windowHeight="18684" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="パーツ一覧" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="356">
   <si>
     <t>パーツ一覧</t>
   </si>
@@ -1977,31 +1977,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Data1</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Data2</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Data3</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>[4]</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>[5]</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Step Timing</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Is Repeat</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -2519,12 +2499,279 @@
     <t>Set Step Timing</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>[6]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Step Timing (H)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Step Timing (L)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0～65535</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Step Timing
+(2byte)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Pattern Flags</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Repeat=1 で無限リピート
+Inverse=1 でパターンの 1 と 0 を反転</t>
+    <rPh sb="10" eb="12">
+      <t>ムゲン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ハンテン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>bit0 : Repeat
+bit1 : Inverse
+bit2-7 : (Reserved)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* ステップ周期 (単位は ms)
+* ビッグエンディアンで格納</t>
+    <rPh sb="6" eb="8">
+      <t>シュウキ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>タンイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクノウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■StepTiming の 2byte 化について</t>
+    <rPh sb="20" eb="21">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* 上限で 1 Step 1 秒くらいまでパターンをゆっくりにさせたい。</t>
+    <rPh sb="2" eb="4">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ビョウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* 下限近くでは LED の速度変化が大きく表れるので細かく制御したい。</t>
+    <rPh sb="2" eb="4">
+      <t>カゲン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ソクド</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>コマ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セイギョ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* 最初は 1byte で考えていたが、0-255ms だと遅い方の表現力に不満がある。</t>
+    <rPh sb="2" eb="4">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>カンガ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>オソ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ヒョウゲン</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>リョク</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>フマン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* 一方で下限近くを 1ms で細かく制御できるのは無駄なので値に傾斜をかける案はあった。(0~N: 1msずつ、N+1~255: 5ms ずつ、など)</t>
+    <rPh sb="2" eb="4">
+      <t>イッポウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カゲン</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>コマ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>セイギョ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ムダ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ケイシャ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>アン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* しかし↑のようにするとツール側での指定が、その傾斜に依存して試行錯誤がやりにくくなる懸念があった。</t>
+    <rPh sb="16" eb="17">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ケイシャ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>イゾン</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>シコウ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>サクゴ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ケネン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>□要求：</t>
+    <rPh sb="1" eb="3">
+      <t>ヨウキュウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>□1byte にしなかった理由</t>
+    <rPh sb="13" eb="15">
+      <t>リユウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>⇒ 現状、I2C の通信速度が足りてないわけではないのでファームウェア側にむやみに制約をつけるのは望ましくないと判断。</t>
+    <rPh sb="2" eb="4">
+      <t>ゲンジョウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ツウシン</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ソクド</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>セイヤク</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>ノゾ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ハンダン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>■Pattern Flags について</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* 最初は IsRepeat (無限リピート) しかなかったが、拡張性を考えてフラグに変更。</t>
+    <rPh sb="2" eb="4">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ムゲン</t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t>カクチョウセイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>カンガ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>* Inverse は完全に思いつき。使うかどうかは未定。</t>
+    <rPh sb="11" eb="13">
+      <t>カンゼン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ミテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="游ゴシック"/>
@@ -2594,6 +2841,13 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2627,7 +2881,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2748,11 +3002,35 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2866,6 +3144,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2939,6 +3238,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6043,7 +6345,7 @@
         <v>162</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.4">
@@ -6059,7 +6361,7 @@
         <v>163</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -6142,7 +6444,7 @@
         <v>168</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.4">
@@ -7611,9 +7913,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E918656-40EA-4B26-9256-33A6570B993C}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.4"/>
   <cols>
@@ -7623,51 +7927,51 @@
     <col min="5" max="5" width="24.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="18.21875" style="4" customWidth="1"/>
-    <col min="8" max="9" width="16.109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="4"/>
+    <col min="8" max="10" width="16.109375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B3" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="C4" s="4" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B3" s="4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="C5" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C4" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C5" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C8" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C9" s="4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C10" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="D12" s="35" t="s">
         <v>280</v>
       </c>
@@ -7681,33 +7985,33 @@
         <v>287</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+        <v>289</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="D13" s="35" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>301</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>288</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>289</v>
-      </c>
-      <c r="I13" s="35" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+        <v>296</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="D14" s="13" t="s">
         <v>283</v>
       </c>
@@ -7720,203 +8024,312 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="D15" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="D16" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+        <v>290</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="I16" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D17" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>286</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D18" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="H18" s="37"/>
+        <v>333</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>337</v>
+      </c>
       <c r="I18" s="37"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D19" s="36"/>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
       <c r="G19" s="36"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D21" s="35" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="86.4" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:10" ht="86.4" x14ac:dyDescent="0.4">
       <c r="D22" s="2" t="s">
         <v>283</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="H22" s="40" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+        <v>329</v>
+      </c>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="2:10" ht="28.8" x14ac:dyDescent="0.4">
       <c r="D23" s="2" t="s">
         <v>284</v>
       </c>
       <c r="E23" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="57.6" x14ac:dyDescent="0.4">
+      <c r="D24" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>331</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
-      <c r="D24" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>336</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="57.6" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:10" ht="57.6" x14ac:dyDescent="0.4">
       <c r="D25" s="2" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="28.8" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.4">
       <c r="D26" s="2" t="s">
         <v>286</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B29" s="4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="D30" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:10" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="D27" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="G27" s="46"/>
+    </row>
+    <row r="28" spans="2:10" ht="43.2" x14ac:dyDescent="0.4">
+      <c r="D28" s="45" t="s">
+        <v>340</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B30" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D31" s="39" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D32" s="39" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D33" s="39" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B36" s="4" t="s">
-        <v>324</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D34" s="39" t="s">
+        <v>315</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C37" s="4" t="s">
-        <v>325</v>
+      <c r="B37" s="4" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C38" s="4" t="s">
-        <v>326</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C39" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B42" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="C42" s="47"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B44" s="47"/>
+      <c r="C44" s="47" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B45" s="47"/>
+      <c r="C45" s="47" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B47" s="47"/>
+      <c r="C47" s="47" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B48" s="47"/>
+      <c r="C48" s="47" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B49" s="47"/>
+      <c r="C49" s="47" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B50" s="47"/>
+      <c r="C50" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B51" s="47"/>
+      <c r="C51" s="47" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B54" s="47" t="s">
+        <v>353</v>
+      </c>
+      <c r="C54" s="47"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B55" s="47"/>
+      <c r="C55" s="47" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B56" s="47"/>
+      <c r="C56" s="47" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>